<commit_message>
Se agrega función Agregar datos en archivo excel
Se agrega función para agregar datos  póliza en excel
</commit_message>
<xml_diff>
--- a/e2e/Emision_Autos/Default.xlsx
+++ b/e2e/Emision_Autos/Default.xlsx
@@ -533,10 +533,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
@@ -545,14 +545,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,8 +851,8 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:BD3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -878,7 +878,7 @@
     <col min="57" max="16384" width="9.078125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1">
+    <row r="1" s="11" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1044,7 @@
       <c r="BC1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BD1" s="11" t="s">
+      <c r="BD1" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1094,7 +1094,7 @@
       <c r="O2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="Q2" s="2" t="s">
@@ -1142,7 +1142,7 @@
       <c r="AE2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="AG2" s="2" t="s">
@@ -1160,7 +1160,7 @@
       <c r="AK2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" s="5" t="s">
         <v>101</v>
       </c>
       <c r="AM2" s="3" t="s">
@@ -1185,7 +1185,7 @@
         <v>19</v>
       </c>
       <c r="AT2" s="10">
-        <v>45458</v>
+        <v>45461</v>
       </c>
       <c r="AU2" s="3" t="s">
         <v>65</v>
@@ -1264,7 +1264,7 @@
       <c r="O3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="Q3" s="2" t="s">
@@ -1312,7 +1312,7 @@
       <c r="AE3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AF3" s="5" t="s">
+      <c r="AF3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AG3" s="2" t="s">
@@ -1330,7 +1330,7 @@
       <c r="AK3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AL3" s="5" t="s">
+      <c r="AL3" s="4" t="s">
         <v>101</v>
       </c>
       <c r="AM3" s="3" t="s">
@@ -1354,8 +1354,8 @@
       <c r="AS3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AT3" s="8">
-        <v>45458</v>
+      <c r="AT3" s="9">
+        <v>45461</v>
       </c>
       <c r="AU3" s="3" t="s">
         <v>65</v>

</xml_diff>